<commit_message>
Another set of data added for firsdt test case
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>FirstName</t>
   </si>
@@ -65,6 +65,24 @@
   </si>
   <si>
     <t>Telangana</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Rddy</t>
+  </si>
+  <si>
+    <t>Myadd2</t>
+  </si>
+  <si>
+    <t>Amaravathi</t>
+  </si>
+  <si>
+    <t>ap</t>
   </si>
 </sst>
 </file>
@@ -417,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,9 +517,42 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3">
+        <v>123456</v>
+      </c>
+      <c r="I3">
+        <v>1234567899</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>